<commit_message>
Daten umsetzen in Excel
</commit_message>
<xml_diff>
--- a/PA_Primardaten_Sensor 2.xlsx
+++ b/PA_Primardaten_Sensor 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenwei/Desktop/PA 表格处理/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenwei/Desktop/PA_Daten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3105EF53-7A20-594F-89BD-E141ED2D38A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A36A79-1A87-0447-8157-C8B91AD46D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="17100" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variante(T1)" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>Sensor2</t>
   </si>
@@ -339,6 +339,14 @@
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>Geschwindigkeit</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abstand(Streck)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -347,7 +355,7 @@
   <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0.0000_ "/>
-    <numFmt numFmtId="182" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="178" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -657,6 +665,22 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -675,30 +699,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="182" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3710,6 +3718,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1902406912"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -11874,8 +11883,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>37820</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="25" name="墨迹 24">
@@ -11894,7 +11903,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="25" name="墨迹 24">
@@ -11939,8 +11948,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>86560</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="45" name="墨迹 44">
@@ -11959,7 +11968,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="45" name="墨迹 44">
@@ -11981,71 +11990,6 @@
             <a:xfrm>
               <a:off x="8940600" y="5123160"/>
               <a:ext cx="36000" cy="36000"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>528480</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>97280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>754900</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>63200</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="62" name="墨迹 61">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C27785F1-BDC5-3823-BD3D-CED06B558929}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="15387480" y="2510280"/>
-            <a:ext cx="1051920" cy="956520"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="62" name="墨迹 61">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C27785F1-BDC5-3823-BD3D-CED06B558929}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="15369840" y="2492640"/>
-              <a:ext cx="1087560" cy="992160"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -12238,8 +12182,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>59500</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="4" name="墨迹 3">
@@ -12258,7 +12202,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="4" name="墨迹 3">
@@ -12363,33 +12307,6 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2022-10-09T20:54:04.737"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.1" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2468 1362 8191,'-5'9'0,"1"-4"5063,4 11-5063,0 12 0,0-3 0,0 21 0,0-34 0,0 22 0,0-28 0,0 35 0,0-21 0,0 21 2818,0-11-2818,0-1 0,0-9 0,0-3 1719,0-12-1719,0-1 6784,0-12-6784,0 7 0,0-53 0,0 29 0,0-52 0,0 49-3325,10-36 1,3-4 3324,-3 15 0,11-25 0,0 2-1071,-8 35 1071,10-23 0,1 0 0,-9 21-2114,16-46 1,0-1 2113,-14 43 0,19-46 0,1 5-549,-22 56 549,11-26 0,1-2 0,-8 18 0,11-30 0,2 11 0,0 1 0,-8 14 0,-4 4 0,-3 11 3522,-1 3-3522,-3 9 967,-2 2-967,-3 6 6178,-1 2-6178,4 3 1283,-2 2-1283,5 4 546,-2 0-546,8 0 0,-6 0 0,10 0 0,-7 0 0,12 3 0,-10 0 0,19 12 0,-10-3 0,24 23 0,16 18 0,-11-5-3392,-10-3 0,1 4 3392,15 24 0,-30-33 0,0 1-446,-2 10 1,-3-2 445,0 0 0,-6 8 0,-2 1 0,-2-6 0,0 10 0,0 2 0,0-2 0,-5 1 0,-2-2 0,0-7 0,-4 10 0,-1-1 0,-2-23 0,0 13 0,-1-3 0,-2-25 0,-1 58 0,0-58 0,0 69 0,0-72 0,0 68 0,0-56 0,0 36 0,0-9 0,-5-12 0,-2 15 0,1-29 0,0-5 0,6-12 0,0-3 6343,-2-3-6343,-1-3 1332,1-1-1332,0-2 0,2 3 0,0-3 0,0-7 0,0-19 0,0 3 0,10-42 0,-4 31-2164,13-21 1,4-3 2163,-1 4 0,11-20 0,1 0 0,-7 13 0,6-2 0,-1 2-1290,-10 19 1290,16-26 0,0-1 0,-13 18-907,7-8 1,6-12-1,-5 10 907,-1 3 0,22-29 0,1 4 0,-25 36 0,8-8 0,-2 3-238,-20 26 238,40-56 0,-26 41 2315,26-34-2315,-26 35 0,-2 2 0,-9 10 0,-1 0 0,-3 8 1234,-2 0-1234,-2 6 0,-2 1 0,2 4 3461,-2 1-3461,5 2 378,-1 0-378,2 0 1187,-4 0-1187,4 6 0,-3-1 0,13 21 0,-5-5 0,9 29 0,-8-13 0,11 32 0,-9-21-773,12 37 773,-13-29-710,-8-1 1,0 2 709,2 13 0,-4-4 0,0 1 0,2 8-955,-4-2 0,-1 0 955,0 5 0,-2 3 0,0 0 0,-1-3 0,-2 0 0,-1-2 0,-1-7 0,-1-16 0,-2-3 0,1-10 0,0 43 0,0-47 0,0 58 0,0-61 0,0 40 0,0-51 0,0 43-1404,0-47 1404,0 35 0,0-41 0,-4 27 147,2-30 0,-3 11 0,4-18 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
       <inkml:timestamp xml:id="ts0" timeString="2022-10-09T20:55:40.459"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
@@ -12400,10 +12317,6 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">0 272 24575,'45'-5'0,"-2"1"0,13 4 0,-18 0 0,24 0 0,14 0 0,-5 0-792,-15 0 1,-2 0 791,-6 0 0,4 0 0,1 0 0,-5 0 0,10 0 0,0 0 0,-8 0 0,11 0 0,-1 0 0,-15 0 0,18 0 0,0 0 0,-21 0 0,23 0 0,0 0 0,-20 0-619,16 0 1,16 0 0,-12 0 618,1 0 0,12 0 0,18 0 0,-20 0 0,-22 0 0,21 0 0,19 0 0,-20 0 0,-25 0 0,12 0 0,21 0 0,13 0 0,5 0 0,-22 0 0,8 0 0,5 0 0,4 0 0,1 0 0,-3 0 0,-3 0 0,-7 0-1129,11 0 0,-9 0 0,-1 0 0,3 0 0,11 0 1129,-11 0 0,11 0 0,8 0 0,3 0 0,0 0 0,-4 0 0,-9 0 0,-11 0 0,-16 0-1888,27 0 0,-14 0 1888,-2 0 0,4 0 0,-7 0-500,-1 0 1,-2 0 499,-4 0 0,5 0 0,-3 0-473,21 0 0,3 0 473,-20 0 0,8 0 0,0 0 0,-8 0 0,24 0 0,-2 0 0,-10-4 0,5 0 0,-6-1 0,5 0 0,-5-1 0,13-4 0,-4-1 0,-31 4 0,-1 1 0,13 2 0,-3 1 0,16 0 0,-15 0 0,-1-1 0,22-1 0,2 1 0,1 1 0,-43 1 0,-1 1 0,35 0 0,-2 2 0,4-1 0,-14 0 0,0 0 0,4 0 0,-5 0 0,-1 0 0,-5 0 0,3 0 0,-1 0 0,-12 0 0,6 0 0,-2 0 2405,-18 0-2405,8 0 0,0 0 0,-14 0 0,10 0 0,0 0 0,-14 0 0,51 0 0,-52 0 0,58 0 0,-60 0 0,20 0 0,-2 0 0,-30 0 0,30-3 0,4-1 0,-8 2 0,43-5 0,-39 7 0,-6 0 0,-3 0 0,-1 0 0,14 0 3698,-7 0-3698,20 0 0,-16 0 0,10 0 0,-8 0 0,-9 0 0,7 0 0,-12 0 0,1 0 0,-10 0 0,11 0 0,-11 0 0,17 0 0,-14 0 0,9 0 0,-14 0 0,15 0 0,12 0 0,10 0 0,-5 0 0,-11 0 0,-27 0 0,8 0 0,-16 0 0,16 0 2621,-16 0-2621,12 4 4610,-16-3-4610,28 4 0,-28-4 0,39 3 0,-37-2 0,23 8 0,-26-8 0,22 3 0,-25-5 0,32 5 953,-32-3-953,21 3 0,-25-5 0,16 0 517,-10 2-517,8 1 0,19 0 0,-20 2 0,18-3 0,-22 1 0,0-1 0,5-2 0,-3 0 0,0 3 0,-3-1 0,-4 1 0,-2-1 0,-1-2 0,-1 0 0,1 0 0,-1 0 0,2 3 0,-3-1 0,3 1 0,-3-2 0,3-1 0,-3 0 0,0 0 0,-2 0 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1786">5649 51 24575,'-12'13'0,"-13"16"0,-23 34 0,9-12 0,-3 3-4916,6-7 1,-1 1 4408,-10 17 1,-3 3 506,-4 1 0,2-2-1195,13-15 0,1 2 1195,-22 26 0,6-7 0,20-27 621,-9 18 0,2-2-621,11-19 0,-6 9 0,-9 11 0,7-11 0,2-2 0,-3 5 0,-9 12 0,10-14 0,10-14 0,-9 20 0,-2 1 0,6-12 0,-16 29 0,21-35 0,0 2-2812,-24 38 2812,25-35 0,2-2 0,-7 7 2599,6-8-2599,14-27 0,1 0 0,1 5 0,3-4 4099,1-3-4099,1-3 1322,-1-1-1322,2-2 6784,-2 0-6784,2-4 0,1 0 0,2-1 0,1 2 0,0-3 0,3 1 0,-2-4 0,7 0 0,-3 0 0,5 0 0,0 0 0,0 0 0,3 0 0,0 0 0,5 0 0,35-12 0,-13 5 0,25-9 0,-6 7 0,-11 3-908,36 1 908,-16 2-1258,-2 0 1,3 0 1257,-15 0 0,0 1 0,13-2 0,-3 1 0,21-1 0,11 4 0,-25 0 0,-7 0 0,7 0 0,0 0 0,-1 0 0,-9 0 0,-2 0 0,2 0 0,-3 0 0,16 0 0,-18 0 0,16 0-1831,9 0 1831,-27 0 0,32 0-224,-55 0 224,13 0 2211,-31 0-2211,17 0 0,-19 0 0,26 0 0,-26 0 0,57 0 0,-45 0 0,52 0 0,-57 0 0,27 0 0,-34 0 0,37 0-4317,-38 0 4317,38 0-1267,-26 0 1267,16 0 0,19-6 0,-18-1 0,13-3 0,-24 1 0,0 6 0,-9-2 5760,1 2-5760,-12-2 3091,-2 1-3091,-1 1 0,-1 1 0,1-1 0,-1 1 0,-1-3 0,-2 1 0,-1-1 0,0-2 0,0 2 0,0-3 0,0 5 0,0-3 0,0 3 0,0-3 0,0 3 0,0-3 0,-3 0 0,1 1 0,-5-7 0,5 7 0,-10-6 0,8 8 0,-11-9 0,10 8 0,-7-8 0,9 10 0,-23-25 0,19 21 0,-57-58 0,52 51-2127,-32-38 1,0-2 2126,30 35 0,-39-46 0,-9-11 0,5 6 0,2 5 0,-2-3 0,12 9 0,3 2 0,1 4 0,2-1 0,4 3 0,2 1 0,4 7 0,0 0 0,-3-5 0,-1-1 0,3 5 0,-1-2 0,-12-17 0,-1-2 0,8 11 0,1 1 0,5 7 0,2 3 0,-14-20-639,-3 4 639,7 9 0,-16-25 0,15 20 0,0 2 0,10 15 0,3 6 0,7 9 0,0 0 0,8 9 0,1-4 0,4 7 0,0 1 4086,3 4-4086,-3-1 806,2 2-806,1-2 0,2 3 0,1-1 0</inkml:trace>
 </inkml:ink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13497,12 +13410,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.75" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
     </row>
     <row r="2" spans="1:4" ht="32.25" customHeight="1">
       <c r="A2" s="1"/>
@@ -13566,7 +13479,7 @@
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 VERTRAULICH</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -13582,72 +13495,72 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="5" spans="3:16">
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
     </row>
     <row r="6" spans="3:16">
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
     </row>
     <row r="7" spans="3:16">
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
     </row>
     <row r="8" spans="3:16">
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
     </row>
     <row r="9" spans="3:16">
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
     </row>
     <row r="10" spans="3:16">
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13655,6 +13568,9 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 VERTRAULICH</oddFooter>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -13667,10 +13583,10 @@
   <dimension ref="A1:AJ92"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="112" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="W6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AB5" sqref="AB5"/>
+      <selection pane="bottomRight" activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
@@ -13682,43 +13598,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="31" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="Z1" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB1" s="22" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="2" spans="1:36" ht="20.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="34" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="34" t="s">
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -13747,30 +13669,30 @@
     </row>
     <row r="3" spans="1:36" ht="20.25" customHeight="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="38" t="s">
+      <c r="G3" s="42"/>
+      <c r="H3" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38" t="s">
+      <c r="I3" s="42"/>
+      <c r="J3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="38" t="s">
+      <c r="K3" s="42"/>
+      <c r="L3" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="37"/>
+      <c r="M3" s="42"/>
       <c r="N3" s="23" t="s">
         <v>36</v>
       </c>
@@ -16105,7 +16027,7 @@
         <v>-0.37549238822504694</v>
       </c>
       <c r="AH26" s="14">
-        <f t="shared" ref="AH25:AH41" si="56">-(AG7+90-AG26)</f>
+        <f t="shared" ref="AH26:AH40" si="56">-(AG7+90-AG26)</f>
         <v>-0.3243639872837949</v>
       </c>
     </row>
@@ -18455,7 +18377,7 @@
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 VERTRAULICH</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -19129,6 +19051,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 VERTRAULICH</oddFooter>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -19137,7 +19062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D11BD6-8C99-7B4D-A43C-B7AD518462D7}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="93" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="93" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:G51"/>
     </sheetView>
   </sheetViews>
@@ -19184,7 +19109,7 @@
         <v>-0.12</v>
       </c>
       <c r="G3" s="17">
-        <f t="shared" ref="G3:G53" si="0">_xlfn.NORM.DIST(F3,$B$10,$C$10,FALSE)</f>
+        <f t="shared" ref="G3:G51" si="0">_xlfn.NORM.DIST(F3,$B$10,$C$10,FALSE)</f>
         <v>2.0173485366054602E-4</v>
       </c>
     </row>
@@ -19805,6 +19730,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 VERTRAULICH</oddFooter>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -19820,219 +19748,219 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:11" ht="14">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:11" ht="14" customHeight="1">
-      <c r="A2" s="42"/>
-      <c r="B2" s="45" t="s">
+      <c r="A2" s="34"/>
+      <c r="B2" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="42"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="42"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="42"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
     </row>
     <row r="6" spans="1:11" ht="14">
-      <c r="A6" s="42"/>
-      <c r="B6" s="42" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42" t="s">
+      <c r="G6" s="34"/>
+      <c r="H6" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="34"/>
     </row>
     <row r="7" spans="1:11" ht="14">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="35">
         <v>-2.43333E-5</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="35">
         <v>2.1926E-5</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="37">
         <v>11.688000000000001</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42">
+      <c r="E7" s="34"/>
+      <c r="F7" s="34">
         <v>1000</v>
       </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42">
+      <c r="G7" s="34"/>
+      <c r="H7" s="34">
         <v>250</v>
       </c>
-      <c r="I7" s="42"/>
+      <c r="I7" s="34"/>
     </row>
     <row r="8" spans="1:11" ht="14">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="36">
         <v>-7.96E-6</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="35">
         <v>-4.1479999999999999E-6</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="37">
         <v>12.055999999999999</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42">
+      <c r="E8" s="34"/>
+      <c r="F8" s="34">
         <v>1000</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42">
+      <c r="G8" s="34"/>
+      <c r="H8" s="34">
         <v>250</v>
       </c>
-      <c r="I8" s="42"/>
+      <c r="I8" s="34"/>
     </row>
     <row r="9" spans="1:11" ht="14">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="43">
+      <c r="B9" s="35">
         <v>-1.5296300000000001E-5</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="35">
         <v>7.1111000000000004E-6</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="37">
         <v>11.817299999999999</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42">
+      <c r="E9" s="34"/>
+      <c r="F9" s="34">
         <v>1000</v>
       </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42">
+      <c r="G9" s="34"/>
+      <c r="H9" s="34">
         <v>250</v>
       </c>
-      <c r="I9" s="42"/>
+      <c r="I9" s="34"/>
     </row>
     <row r="10" spans="1:11" ht="14">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="43">
+      <c r="B10" s="35">
         <v>-2.3148099999999999E-5</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="35">
         <v>1.1852000000000001E-6</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="37">
         <v>11.985300000000001</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42">
+      <c r="E10" s="34"/>
+      <c r="F10" s="34">
         <v>1000</v>
       </c>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42">
+      <c r="G10" s="34"/>
+      <c r="H10" s="34">
         <v>250</v>
       </c>
-      <c r="I10" s="42"/>
+      <c r="I10" s="34"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="42"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="42"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
     </row>
     <row r="13" spans="1:11" ht="14">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="42">
+      <c r="B13" s="34">
         <v>0.58630632400000005</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -20041,6 +19969,9 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 VERTRAULICH</oddFooter>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -20709,6 +20640,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 VERTRAULICH</oddFooter>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -21377,6 +21311,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 VERTRAULICH</oddFooter>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -22045,6 +21982,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 VERTRAULICH</oddFooter>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -22053,8 +21993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD17970-4373-C749-8941-3C2B3516445F}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -22715,6 +22655,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000 VERTRAULICH</oddFooter>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>